<commit_message>
Change DrugCategories to DrugShapes
</commit_message>
<xml_diff>
--- a/database/seeds/files.xlsx
+++ b/database/seeds/files.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Pharmacy\database\seeds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA576F0-08FB-4527-ADE1-2C1358222B97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249EF01B-DB17-478A-BEA2-120205208FE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="companies" sheetId="1" r:id="rId1"/>
-    <sheet name="drug_categories" sheetId="2" r:id="rId2"/>
+    <sheet name="drug_shapes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -819,7 +819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -1239,8 +1239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E752FB2E-DA5F-4E3D-B323-1FD70EB7A242}">
   <dimension ref="A1:A77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>